<commit_message>
store procedure activar , dame y listar rubros
</commit_message>
<xml_diff>
--- a/Documentacion.xlsx
+++ b/Documentacion.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcordoba\Desktop\fondo\Nueva carpeta\CursoDeBasesDeDatosDeAltoRendimiento_Resolucion_Facundo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="20115" windowHeight="8505"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Procedimiento</t>
   </si>
@@ -72,9 +77,6 @@
     <t>_</t>
   </si>
   <si>
-    <t>Mensaje varchar(100), Id smallint</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -87,9 +89,6 @@
     <t>ssp_alta_rubro</t>
   </si>
   <si>
-    <t>pCuenta varchar(60), pIdCategoria smallint, pCategoria varchar(60), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
-  </si>
-  <si>
     <t>Mensaje varchar(100)</t>
   </si>
   <si>
@@ -100,6 +99,36 @@
   </si>
   <si>
     <t>GestorRubros.php</t>
+  </si>
+  <si>
+    <t>ssp_listar_rubros</t>
+  </si>
+  <si>
+    <t>Permite listar los rubros de los productos ordenados por nombre .</t>
+  </si>
+  <si>
+    <t>{Campos de la Tabla Rubros}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Procedimiento que sirve para instanciar un rubro desde la base de datos.</t>
+  </si>
+  <si>
+    <t>ssp_dame_rubro</t>
+  </si>
+  <si>
+    <t>pIdRubro tinyint</t>
+  </si>
+  <si>
+    <t>Mensaje varchar(100), Id tinyint</t>
+  </si>
+  <si>
+    <t>pCuenta varchar(60), pIdRubro tinyint, pNombreRubro varchar(30), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>ssp_activar_rubro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite cambiar el estado del rubro  a A: Activo siempre y cuando no  esté activo ya. Devuelve OK o el mensaje de error en Mensaje. </t>
   </si>
 </sst>
 </file>
@@ -134,7 +163,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,12 +174,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA4C2F4"/>
         <bgColor rgb="FFA4C2F4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -221,23 +244,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -249,6 +269,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,6 +282,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -307,7 +333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,7 +368,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +643,7 @@
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -634,64 +660,151 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="H4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="6" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="19" t="s">
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
auditorias rubros, primeros sp de las tablas personas proveedores y personas
</commit_message>
<xml_diff>
--- a/Documentacion.xlsx
+++ b/Documentacion.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcordoba\Desktop\fondo\Nueva carpeta\CursoDeBasesDeDatosDeAltoRendimiento_Resolucion_Facundo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="120" yWindow="165" windowWidth="20115" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Procedimiento</t>
   </si>
@@ -83,9 +78,6 @@
     <t>Permite dar de alta un rubro, controlando que el nombre no exista ya. Lo da de alta  con estado A: Activo. Devuelve OK + Id o el mensaje de error en Mensaje.</t>
   </si>
   <si>
-    <t>pCuenta varchar(60), pNombreRubro varchar(30), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
-  </si>
-  <si>
     <t>ssp_alta_rubro</t>
   </si>
   <si>
@@ -122,20 +114,114 @@
     <t>Mensaje varchar(100), Id tinyint</t>
   </si>
   <si>
-    <t>pCuenta varchar(60), pIdRubro tinyint, pNombreRubro varchar(30), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
-  </si>
-  <si>
     <t>ssp_activar_rubro</t>
   </si>
   <si>
     <t xml:space="preserve">Permite cambiar el estado del rubro  a A: Activo siempre y cuando no  esté activo ya. Devuelve OK o el mensaje de error en Mensaje. </t>
+  </si>
+  <si>
+    <t>ssp_borra_rubro</t>
+  </si>
+  <si>
+    <t>pNombreRubro varchar(30),pCuenta varchar(60), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>Permite borrar un rubro controlando que no tenga productos asociadas. Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>pIdRubro tinyint,pCuenta varchar(60), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>pIdRubro tinyint, pNombreRubro varchar(30), pCuenta varchar(60), 
+        pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ssp_listar_persona</t>
+  </si>
+  <si>
+    <t>Permite listar las peronas ordenados por nombre.</t>
+  </si>
+  <si>
+    <t>{Campos de la Tabla Personas}</t>
+  </si>
+  <si>
+    <t>GestorPersonas.php</t>
+  </si>
+  <si>
+    <t>ssp_activar_persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite cambiar el estado de una persona   a A: Activo siempre y cuando no  esté activo ya. Devuelve OK o el mensaje de error en Mensaje. </t>
+  </si>
+  <si>
+    <t>ssp_inactivar_persona</t>
+  </si>
+  <si>
+    <t>ssp_inactivar_rubro</t>
+  </si>
+  <si>
+    <t>Permite cambiar el estado de el rubro a I: inactivo  siempre y cuando no 
+    esté Inactivo y no existan productos asociadas en estado activo. 
+    Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>pIdRubro  tinyint</t>
+  </si>
+  <si>
+    <t>Permite cambiar el estado de la persona  a I: inactiva siempre y cuando no 
+    esté Inactiva 
+    Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>ssp_alta_persona</t>
+  </si>
+  <si>
+    <t>Mensaje varchar(100), Id int</t>
+  </si>
+  <si>
+    <t>Permite dar de alta una persona controlando que el nombre y el telefono no sean vacios , ni  NULOS. La da de alta  con estado A: Activa. Devuelve OK  + Id o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>ssp_modifica_persona</t>
+  </si>
+  <si>
+    <t>Permite modificar una persona existente, controlando que el nombre y el telefono no sean vacios , ni  NULO. Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>pNombres varchar(30),pTelefono char (10)</t>
+  </si>
+  <si>
+    <t>pIdPersonas int</t>
+  </si>
+  <si>
+    <t>pIdPersonas int, pNombres varchar(30),pTelefono char (10)</t>
+  </si>
+  <si>
+    <t>ssp_alta_proveedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite dar de alta un proveedor controlando que el nombre y el telefono no sean vacios , ni  NULOS. 
+La da de alta  con estado A: Activa. Devuelve OK  + Id o el mensaje de error en Mensaje </t>
+  </si>
+  <si>
+    <t>GestorProveedores.php</t>
+  </si>
+  <si>
+    <t>ssp_modifica_proveedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Permite modificar un proveedor existente, controlando que el nombre y el telefono no sean vacios , ni  NULO.
+    Devuelve OK o el mensaje de error en Mensaje.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +248,21 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,12 +277,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -219,29 +330,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -257,19 +421,50 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -333,7 +528,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,7 +563,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -577,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,223 +783,496 @@
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="E4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="H8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="18" t="s">
+      <c r="F9" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="H9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="D10" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se crearon las auditorias nivel 2 para personas, rubros, proveedores y nivel 2 para ventas
</commit_message>
<xml_diff>
--- a/Documentacion.xlsx
+++ b/Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="88">
   <si>
     <t>Procedimiento</t>
   </si>
@@ -54,16 +54,10 @@
     <t>OK</t>
   </si>
   <si>
-    <t>ssp_listar_tiposroles</t>
-  </si>
-  <si>
     <t>{Campos de la Tabla Roles}</t>
   </si>
   <si>
     <t>GestorEmpleados.php</t>
-  </si>
-  <si>
-    <t>Permite listar los tipos de roles de un empleado ordenados por tipo rol.</t>
   </si>
   <si>
     <t>Empleado</t>
@@ -137,9 +131,6 @@
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>ssp_listar_persona</t>
   </si>
   <si>
     <t>Permite listar las peronas ordenados por nombre.</t>
@@ -197,9 +188,6 @@
     <t>pIdPersonas int</t>
   </si>
   <si>
-    <t>pIdPersonas int, pNombres varchar(30),pTelefono char (10)</t>
-  </si>
-  <si>
     <t>ssp_alta_proveedor</t>
   </si>
   <si>
@@ -215,6 +203,92 @@
   <si>
     <t xml:space="preserve">   Permite modificar un proveedor existente, controlando que el nombre y el telefono no sean vacios , ni  NULO.
     Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>ssp_borra_proveedor</t>
+  </si>
+  <si>
+    <t>Permite borrar un proveedor controlando que no tenga compras asociadas. Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>pIdProveedor int, pCuenta varchar(60), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>ssp_dame_proveedor</t>
+  </si>
+  <si>
+    <t>pIdProveedor int</t>
+  </si>
+  <si>
+    <t>{Campos de la Tabla Proveedores}</t>
+  </si>
+  <si>
+    <t>Permite listar los proveedores ordenados por nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Procedimiento que sirve para instanciar un proveedor desde la base de datos o  o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>ssp_listar_personas</t>
+  </si>
+  <si>
+    <t>ssp_listar_proveedores</t>
+  </si>
+  <si>
+    <t>ssp_listar_roles</t>
+  </si>
+  <si>
+    <t>Permite listar los roles de un empleado ordenados por tipo rol.</t>
+  </si>
+  <si>
+    <t>pNombres varchar(30),pTelefono char (10), pCuenta varchar(60), pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>pIdPersonas int, pNombres varchar(30),pTelefono char (10),pCuenta varchar(60), 
+        pIP varchar(40), pUserAgent varchar(255), pAplicacion varchar(50)</t>
+  </si>
+  <si>
+    <t>pIdProveedor int, pNombres varchar(30),pTelefono char (10)</t>
+  </si>
+  <si>
+    <t>ssp_alta_venta</t>
+  </si>
+  <si>
+    <t>Permite dar de alta una venta controlando que la fecha y hora no exista ya y sean unicas . Devuelve OK + Id o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>pIdCliente int, pIdEmpleado int, FechaVenta dateTime</t>
+  </si>
+  <si>
+    <t>GestorVentas.php</t>
+  </si>
+  <si>
+    <t>ssp_modifica_venta</t>
+  </si>
+  <si>
+    <t>pIdVenta bigint, pFechaVenta dateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Permite modificar la fecha de una venta existente, controlando que la fecha no este vacia , ni  nula.
+    Devuelve OK o el mensaje de error en Mensaje.</t>
+  </si>
+  <si>
+    <t>ssp_listar_ventas</t>
+  </si>
+  <si>
+    <t>Permite listar las ventas ordenados por FechaVenta</t>
+  </si>
+  <si>
+    <t>{Campos de la Tabla Ventas}</t>
+  </si>
+  <si>
+    <t>pIdVenta bigint</t>
+  </si>
+  <si>
+    <t>ssp_dame_venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Procedimiento que sirve para instanciar una venta desde la base de datos   o el mensaje de error en Mensaje.</t>
   </si>
 </sst>
 </file>
@@ -262,7 +336,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +364,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,6 +547,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -827,19 +908,19 @@
     </row>
     <row r="2" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>10</v>
@@ -856,25 +937,25 @@
     </row>
     <row r="3" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>11</v>
@@ -887,25 +968,25 @@
     </row>
     <row r="4" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>11</v>
@@ -918,19 +999,19 @@
     </row>
     <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>10</v>
@@ -947,19 +1028,19 @@
     </row>
     <row r="6" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>10</v>
@@ -976,19 +1057,19 @@
     </row>
     <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -1005,56 +1086,56 @@
     </row>
     <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="C8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H9" s="27" t="s">
         <v>11</v>
@@ -1065,19 +1146,19 @@
     </row>
     <row r="10" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>10</v>
@@ -1094,19 +1175,19 @@
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>10</v>
@@ -1123,25 +1204,25 @@
     </row>
     <row r="12" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F12" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H12" s="27" t="s">
         <v>11</v>
@@ -1152,25 +1233,25 @@
     </row>
     <row r="13" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>11</v>
@@ -1183,25 +1264,25 @@
     </row>
     <row r="14" spans="1:11" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>11</v>
@@ -1214,25 +1295,25 @@
     </row>
     <row r="15" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>11</v>
@@ -1245,25 +1326,25 @@
     </row>
     <row r="16" spans="1:11" ht="100.5" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>11</v>
@@ -1273,6 +1354,217 @@
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="M19" s="33"/>
+    </row>
+    <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" ht="86.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>